<commit_message>
Revert "XLS MODIFY 1"
This reverts commit baad6ec0992e29d39b28649f4836ff3190be7cc7.
</commit_message>
<xml_diff>
--- a/101-103G.xlsx
+++ b/101-103G.xlsx
@@ -503,7 +503,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -538,7 +538,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>